<commit_message>
Added meta-analysis component to project summary
</commit_message>
<xml_diff>
--- a/Data/literature/limit_data.xlsx
+++ b/Data/literature/limit_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/tonsa_infected_CTmax/Data/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E8FB38-468B-944B-A241-95865DCA6262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D0A785-CECB-F343-8D98-C14116734473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{3B64A76D-4FD5-6C4D-8777-97279F300A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="77">
   <si>
     <t>year</t>
   </si>
@@ -65,21 +65,12 @@
     <t>ramp_rate</t>
   </si>
   <si>
-    <t>acc_temp</t>
-  </si>
-  <si>
     <t>infected_mean</t>
   </si>
   <si>
-    <t>infected_se</t>
-  </si>
-  <si>
     <t>uninfected_mean</t>
   </si>
   <si>
-    <t>ninfected_se</t>
-  </si>
-  <si>
     <t>uninfected_N</t>
   </si>
   <si>
@@ -93,6 +84,189 @@
   </si>
   <si>
     <t>host_sex</t>
+  </si>
+  <si>
+    <t>10.1038/s41598-017-09950-3</t>
+  </si>
+  <si>
+    <t>Greenspan et al. 2017</t>
+  </si>
+  <si>
+    <t>Litoria_spenceri</t>
+  </si>
+  <si>
+    <t>Chordata</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Batrachochytrium_dendrobatidis</t>
+  </si>
+  <si>
+    <t>ectoparasite</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>1 C/m</t>
+  </si>
+  <si>
+    <t>acc_treatment</t>
+  </si>
+  <si>
+    <t>15C constant</t>
+  </si>
+  <si>
+    <t>15C pulse</t>
+  </si>
+  <si>
+    <t>18C constant</t>
+  </si>
+  <si>
+    <t>18C pulse</t>
+  </si>
+  <si>
+    <t>onset_of_spasms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1016/j.jtherbio.2007.09.005 </t>
+  </si>
+  <si>
+    <t>Sherman 2008</t>
+  </si>
+  <si>
+    <t>Notophthalmus_viridescens</t>
+  </si>
+  <si>
+    <t>Ichthyophonus_sp</t>
+  </si>
+  <si>
+    <t>protist</t>
+  </si>
+  <si>
+    <t>fungus</t>
+  </si>
+  <si>
+    <t>24C</t>
+  </si>
+  <si>
+    <t>error_type</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>22C</t>
+  </si>
+  <si>
+    <t>Arthropoda</t>
+  </si>
+  <si>
+    <t>arthropod</t>
+  </si>
+  <si>
+    <t>Fernandez-Loras et al. 2017</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0216090</t>
+  </si>
+  <si>
+    <t>0.8 C/m</t>
+  </si>
+  <si>
+    <t>heat_coma</t>
+  </si>
+  <si>
+    <t>18C</t>
+  </si>
+  <si>
+    <t>Only tadpoles from the Toro population included multiple individuals from both the infected and uninfected treatment</t>
+  </si>
+  <si>
+    <t>10.1111/gcb.14713</t>
+  </si>
+  <si>
+    <t>Hector et al. 2019</t>
+  </si>
+  <si>
+    <t>Alytes_obstetricans</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>bacteria</t>
+  </si>
+  <si>
+    <t>endoparasite</t>
+  </si>
+  <si>
+    <t>0.04 C/m</t>
+  </si>
+  <si>
+    <t>20C</t>
+  </si>
+  <si>
+    <t>Daphnia_magna_H</t>
+  </si>
+  <si>
+    <t>Daphnia_magna_M</t>
+  </si>
+  <si>
+    <t>Pasteuria_ramosa_C1</t>
+  </si>
+  <si>
+    <t>Pasteuria_ramosa_C14</t>
+  </si>
+  <si>
+    <t>Pasteuria_ramosa_C20</t>
+  </si>
+  <si>
+    <t>Only one ramping rate was selected</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0198803</t>
+  </si>
+  <si>
+    <t>Agosta et al. 2018</t>
+  </si>
+  <si>
+    <t>Manduca_sexta_fifth_instar</t>
+  </si>
+  <si>
+    <t>0.25 C/m</t>
+  </si>
+  <si>
+    <t>Cotesia_congregata</t>
+  </si>
+  <si>
+    <t>Manduca_sexta_fourth_instar</t>
+  </si>
+  <si>
+    <t>Manduca_sexta_third_instar</t>
+  </si>
+  <si>
+    <t>this_study</t>
+  </si>
+  <si>
+    <t>Sasaki &amp; Dam 2023</t>
+  </si>
+  <si>
+    <t>Acartia_tonsa</t>
+  </si>
+  <si>
+    <t>Probopyrus_sp</t>
+  </si>
+  <si>
+    <t>0.2 C/m</t>
+  </si>
+  <si>
+    <t>uninfected_error</t>
+  </si>
+  <si>
+    <t>infected_error</t>
+  </si>
+  <si>
+    <t>SD calculated from SEM and N reported in study</t>
   </si>
 </sst>
 </file>
@@ -444,15 +618,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDB26D1-83FE-3744-BB20-DAC566B3C133}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -469,7 +647,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -478,7 +656,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -487,28 +665,999 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>2017</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2">
+        <v>37.9</v>
+      </c>
+      <c r="N2">
+        <v>1.7</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="Q2">
+        <v>2.1</v>
+      </c>
+      <c r="R2">
+        <v>11</v>
+      </c>
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>2017</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3">
+        <v>38</v>
+      </c>
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="Q3">
+        <v>2.6</v>
+      </c>
+      <c r="R3">
+        <v>11</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>2017</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4">
+        <v>38.5</v>
+      </c>
+      <c r="N4">
+        <v>1.2</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>34.6</v>
+      </c>
+      <c r="Q4">
+        <v>2.5</v>
+      </c>
+      <c r="R4">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="S4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>2017</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="N5">
+        <v>1.4</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>35.6</v>
+      </c>
+      <c r="Q5">
+        <v>3.1</v>
+      </c>
+      <c r="R5">
+        <v>7</v>
+      </c>
+      <c r="S5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>2008</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6">
+        <v>39.5</v>
+      </c>
+      <c r="N6">
+        <v>0.31622776601700003</v>
+      </c>
+      <c r="O6">
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>38.9</v>
+      </c>
+      <c r="Q6">
+        <v>0.63245553203400007</v>
+      </c>
+      <c r="R6">
+        <v>10</v>
+      </c>
+      <c r="S6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>2017</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7">
+        <v>37</v>
+      </c>
+      <c r="N7">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="O7">
+        <v>39</v>
+      </c>
+      <c r="P7">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="Q7">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="R7">
+        <v>20</v>
+      </c>
+      <c r="S7" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>2019</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8">
+        <v>37.6</v>
+      </c>
+      <c r="N8">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="O8">
+        <v>28</v>
+      </c>
+      <c r="P8">
+        <v>37.4</v>
+      </c>
+      <c r="Q8">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="R8">
+        <v>28</v>
+      </c>
+      <c r="S8" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>2019</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9">
+        <v>37.6</v>
+      </c>
+      <c r="N9">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="O9">
+        <v>28</v>
+      </c>
+      <c r="P9">
+        <v>37.4</v>
+      </c>
+      <c r="Q9">
+        <v>0.501</v>
+      </c>
+      <c r="R9">
+        <v>30</v>
+      </c>
+      <c r="S9" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10">
+        <v>2019</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10">
+        <v>37.6</v>
+      </c>
+      <c r="N10">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="O10">
+        <v>28</v>
+      </c>
+      <c r="P10">
+        <v>37.4</v>
+      </c>
+      <c r="Q10">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="R10">
+        <v>27</v>
+      </c>
+      <c r="S10" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <v>2019</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="N11">
+        <v>0.35</v>
+      </c>
+      <c r="O11">
+        <v>30</v>
+      </c>
+      <c r="P11">
+        <v>37.6</v>
+      </c>
+      <c r="Q11">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="R11">
+        <v>29</v>
+      </c>
+      <c r="S11" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>2019</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="N12">
+        <v>0.35</v>
+      </c>
+      <c r="O12">
+        <v>30</v>
+      </c>
+      <c r="P12">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="Q12">
+        <v>0.38</v>
+      </c>
+      <c r="R12">
+        <v>31</v>
+      </c>
+      <c r="S12" t="s">
+        <v>38</v>
+      </c>
+      <c r="T12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>2019</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="N13">
+        <v>0.35</v>
+      </c>
+      <c r="O13">
+        <v>30</v>
+      </c>
+      <c r="P13">
+        <v>38.1</v>
+      </c>
+      <c r="Q13">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="R13">
+        <v>29</v>
+      </c>
+      <c r="S13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14">
+        <v>2018</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14">
+        <v>44.5</v>
+      </c>
+      <c r="N14">
+        <v>1.4</v>
+      </c>
+      <c r="O14">
+        <v>8</v>
+      </c>
+      <c r="P14">
+        <v>44.1</v>
+      </c>
+      <c r="Q14">
+        <v>1.35</v>
+      </c>
+      <c r="R14">
+        <v>7</v>
+      </c>
+      <c r="S14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15">
+        <v>2018</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15">
+        <v>46.4</v>
+      </c>
+      <c r="N15">
+        <v>1.23</v>
+      </c>
+      <c r="O15">
+        <v>8</v>
+      </c>
+      <c r="P15">
+        <v>45.3</v>
+      </c>
+      <c r="Q15">
+        <v>1.04</v>
+      </c>
+      <c r="R15">
+        <v>5</v>
+      </c>
+      <c r="S15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16">
+        <v>2018</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16">
+        <v>46.4</v>
+      </c>
+      <c r="N16">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="O16">
+        <v>7</v>
+      </c>
+      <c r="P16">
+        <v>45</v>
+      </c>
+      <c r="Q16">
+        <v>2.36</v>
+      </c>
+      <c r="R16">
+        <v>6</v>
+      </c>
+      <c r="S16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>2023</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17">
+        <v>36.6</v>
+      </c>
+      <c r="N17">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O17">
+        <v>20</v>
+      </c>
+      <c r="P17">
+        <v>36.9</v>
+      </c>
+      <c r="Q17">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="R17">
+        <v>17</v>
+      </c>
+      <c r="S17" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-arranged contrasts in forest plot
</commit_message>
<xml_diff>
--- a/Data/literature/limit_data.xlsx
+++ b/Data/literature/limit_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/tonsa_infected_CTmax/Data/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D0A785-CECB-F343-8D98-C14116734473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17D7947-60F0-ED43-B912-93CB656251B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{3B64A76D-4FD5-6C4D-8777-97279F300A7B}"/>
   </bookViews>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDB26D1-83FE-3744-BB20-DAC566B3C133}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,16 +694,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>2017</v>
+        <v>2008</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -712,10 +712,10 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
@@ -727,28 +727,31 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="M2">
-        <v>37.9</v>
+        <v>39.5</v>
       </c>
       <c r="N2">
-        <v>1.7</v>
+        <v>0.31622776601700003</v>
       </c>
       <c r="O2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P2">
-        <v>34.200000000000003</v>
+        <v>38.9</v>
       </c>
       <c r="Q2">
-        <v>2.1</v>
+        <v>0.63245553203400007</v>
       </c>
       <c r="R2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S2" t="s">
         <v>38</v>
+      </c>
+      <c r="T2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -786,22 +789,22 @@
         <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M3">
-        <v>38</v>
+        <v>37.9</v>
       </c>
       <c r="N3">
-        <v>0.9</v>
+        <v>1.7</v>
       </c>
       <c r="O3">
         <v>5</v>
       </c>
       <c r="P3">
-        <v>35.299999999999997</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="Q3">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="R3">
         <v>11</v>
@@ -845,25 +848,25 @@
         <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4">
-        <v>38.5</v>
+        <v>38</v>
       </c>
       <c r="N4">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="O4">
         <v>5</v>
       </c>
       <c r="P4">
-        <v>34.6</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="Q4">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="R4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S4" t="s">
         <v>38</v>
@@ -904,25 +907,25 @@
         <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5">
-        <v>36.200000000000003</v>
+        <v>38.5</v>
       </c>
       <c r="N5">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="O5">
         <v>5</v>
       </c>
       <c r="P5">
-        <v>35.6</v>
+        <v>34.6</v>
       </c>
       <c r="Q5">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="R5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S5" t="s">
         <v>38</v>
@@ -930,16 +933,16 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>2008</v>
+        <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -948,10 +951,10 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
         <v>21</v>
@@ -963,31 +966,28 @@
         <v>23</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M6">
-        <v>39.5</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="N6">
-        <v>0.31622776601700003</v>
+        <v>1.4</v>
       </c>
       <c r="O6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P6">
-        <v>38.9</v>
+        <v>35.6</v>
       </c>
       <c r="Q6">
-        <v>0.63245553203400007</v>
+        <v>3.1</v>
       </c>
       <c r="R6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="S6" t="s">
         <v>38</v>
-      </c>
-      <c r="T6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -1054,188 +1054,179 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C8">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s">
         <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="L8" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="M8">
-        <v>37.6</v>
+        <v>44.5</v>
       </c>
       <c r="N8">
-        <v>0.34300000000000003</v>
+        <v>1.4</v>
       </c>
       <c r="O8">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="P8">
-        <v>37.4</v>
+        <v>44.1</v>
       </c>
       <c r="Q8">
-        <v>0.36499999999999999</v>
+        <v>1.35</v>
       </c>
       <c r="R8">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="S8" t="s">
         <v>38</v>
-      </c>
-      <c r="T8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C9">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="I9" t="s">
         <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="M9">
-        <v>37.6</v>
+        <v>46.4</v>
       </c>
       <c r="N9">
-        <v>0.34300000000000003</v>
+        <v>1.23</v>
       </c>
       <c r="O9">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="P9">
-        <v>37.4</v>
+        <v>45.3</v>
       </c>
       <c r="Q9">
-        <v>0.501</v>
+        <v>1.04</v>
       </c>
       <c r="R9">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="S9" t="s">
         <v>38</v>
-      </c>
-      <c r="T9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C10">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="I10" t="s">
         <v>53</v>
       </c>
       <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10">
+        <v>46.4</v>
+      </c>
+      <c r="N10">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
+      </c>
+      <c r="P10">
         <v>45</v>
       </c>
-      <c r="K10" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M10">
-        <v>37.6</v>
-      </c>
-      <c r="N10">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="O10">
-        <v>28</v>
-      </c>
-      <c r="P10">
-        <v>37.4</v>
-      </c>
       <c r="Q10">
-        <v>0.33500000000000002</v>
+        <v>2.36</v>
       </c>
       <c r="R10">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="S10" t="s">
         <v>38</v>
-      </c>
-      <c r="T10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -1249,7 +1240,7 @@
         <v>2019</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -1276,22 +1267,22 @@
         <v>55</v>
       </c>
       <c r="M11">
-        <v>38.200000000000003</v>
+        <v>37.6</v>
       </c>
       <c r="N11">
-        <v>0.35</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="O11">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P11">
-        <v>37.6</v>
+        <v>37.4</v>
       </c>
       <c r="Q11">
-        <v>0.48499999999999999</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="R11">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S11" t="s">
         <v>38</v>
@@ -1311,7 +1302,7 @@
         <v>2019</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -1338,22 +1329,22 @@
         <v>55</v>
       </c>
       <c r="M12">
-        <v>38.200000000000003</v>
+        <v>37.6</v>
       </c>
       <c r="N12">
-        <v>0.35</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="O12">
+        <v>28</v>
+      </c>
+      <c r="P12">
+        <v>37.4</v>
+      </c>
+      <c r="Q12">
+        <v>0.501</v>
+      </c>
+      <c r="R12">
         <v>30</v>
-      </c>
-      <c r="P12">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="Q12">
-        <v>0.38</v>
-      </c>
-      <c r="R12">
-        <v>31</v>
       </c>
       <c r="S12" t="s">
         <v>38</v>
@@ -1373,7 +1364,7 @@
         <v>2019</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -1400,22 +1391,22 @@
         <v>55</v>
       </c>
       <c r="M13">
-        <v>38.200000000000003</v>
+        <v>37.6</v>
       </c>
       <c r="N13">
-        <v>0.35</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="O13">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P13">
-        <v>38.1</v>
+        <v>37.4</v>
       </c>
       <c r="Q13">
-        <v>0.35499999999999998</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="R13">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S13" t="s">
         <v>38</v>
@@ -1426,179 +1417,188 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C14">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="I14" t="s">
         <v>53</v>
       </c>
       <c r="J14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="N14">
+        <v>0.35</v>
+      </c>
+      <c r="O14">
+        <v>30</v>
+      </c>
+      <c r="P14">
+        <v>37.6</v>
+      </c>
+      <c r="Q14">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="R14">
         <v>29</v>
-      </c>
-      <c r="K14" t="s">
-        <v>65</v>
-      </c>
-      <c r="L14" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14">
-        <v>44.5</v>
-      </c>
-      <c r="N14">
-        <v>1.4</v>
-      </c>
-      <c r="O14">
-        <v>8</v>
-      </c>
-      <c r="P14">
-        <v>44.1</v>
-      </c>
-      <c r="Q14">
-        <v>1.35</v>
-      </c>
-      <c r="R14">
-        <v>7</v>
       </c>
       <c r="S14" t="s">
         <v>38</v>
+      </c>
+      <c r="T14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C15">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="I15" t="s">
         <v>53</v>
       </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="L15" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="M15">
-        <v>46.4</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="N15">
-        <v>1.23</v>
+        <v>0.35</v>
       </c>
       <c r="O15">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="P15">
-        <v>45.3</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="Q15">
-        <v>1.04</v>
+        <v>0.38</v>
       </c>
       <c r="R15">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="S15" t="s">
         <v>38</v>
+      </c>
+      <c r="T15" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C16">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
         <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="I16" t="s">
         <v>53</v>
       </c>
       <c r="J16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="N16">
+        <v>0.35</v>
+      </c>
+      <c r="O16">
+        <v>30</v>
+      </c>
+      <c r="P16">
+        <v>38.1</v>
+      </c>
+      <c r="Q16">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="R16">
         <v>29</v>
-      </c>
-      <c r="K16" t="s">
-        <v>65</v>
-      </c>
-      <c r="L16" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16">
-        <v>46.4</v>
-      </c>
-      <c r="N16">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="O16">
-        <v>7</v>
-      </c>
-      <c r="P16">
-        <v>45</v>
-      </c>
-      <c r="Q16">
-        <v>2.36</v>
-      </c>
-      <c r="R16">
-        <v>6</v>
       </c>
       <c r="S16" t="s">
         <v>38</v>
+      </c>
+      <c r="T16" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
@@ -1661,6 +1661,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T17">
+    <sortCondition ref="C1:C17"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to manuscript files
</commit_message>
<xml_diff>
--- a/Data/literature/limit_data.xlsx
+++ b/Data/literature/limit_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/tonsa_infected_CTmax/Data/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17D7947-60F0-ED43-B912-93CB656251B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84E19D7-515D-B44A-AD4A-6C5130928245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{3B64A76D-4FD5-6C4D-8777-97279F300A7B}"/>
   </bookViews>
@@ -248,9 +248,6 @@
     <t>this_study</t>
   </si>
   <si>
-    <t>Sasaki &amp; Dam 2023</t>
-  </si>
-  <si>
     <t>Acartia_tonsa</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>SD calculated from SEM and N reported in study</t>
+  </si>
+  <si>
+    <t>Sasaki et al. 2023</t>
   </si>
 </sst>
 </file>
@@ -621,7 +621,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,7 +671,7 @@
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O1" t="s">
         <v>11</v>
@@ -680,7 +680,7 @@
         <v>9</v>
       </c>
       <c r="Q1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R1" t="s">
         <v>12</v>
@@ -751,7 +751,7 @@
         <v>38</v>
       </c>
       <c r="T2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1606,13 +1606,13 @@
         <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C17">
         <v>2023</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -1621,7 +1621,7 @@
         <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
         <v>41</v>
@@ -1633,7 +1633,7 @@
         <v>45</v>
       </c>
       <c r="K17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L17" t="s">
         <v>39</v>

</xml_diff>